<commit_message>
Created Gerbs, updated parts to order
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="197">
   <si>
     <t>Qty</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Device</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>R31</t>
   </si>
   <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
     <t>INDUCT-3.2*3.2</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>IC-USB to JTAG</t>
   </si>
   <si>
-    <t>IC-Isolators</t>
-  </si>
-  <si>
     <t>IC-Buck Converter</t>
   </si>
   <si>
@@ -532,6 +523,93 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>100k Resistor (0402)</t>
+  </si>
+  <si>
+    <t>10k Resistor (0402)</t>
+  </si>
+  <si>
+    <t>12k Resistor (0402)</t>
+  </si>
+  <si>
+    <t>1k Resistor (0402)</t>
+  </si>
+  <si>
+    <t>2.2k Resistor (0402)</t>
+  </si>
+  <si>
+    <t>330 Resistor (0402)</t>
+  </si>
+  <si>
+    <t>820 Resistor (0402)</t>
+  </si>
+  <si>
+    <t>0.1u Capacitor (0402)</t>
+  </si>
+  <si>
+    <t>10uf Capacitor (1210)</t>
+  </si>
+  <si>
+    <t>22uf Capacitor (1210)</t>
+  </si>
+  <si>
+    <t>3.3u Capacitor (0402)</t>
+  </si>
+  <si>
+    <t>36p Capacitor (0402)</t>
+  </si>
+  <si>
+    <t>4.7u Capacitor (0402)</t>
+  </si>
+  <si>
+    <t>2.2u Inductor (4012A)</t>
+  </si>
+  <si>
+    <t>2.2u</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>Ferrite Bead-BLM15AG601SN1D  (0402)</t>
+  </si>
+  <si>
+    <t>Ferrite Bead-L-EUL1812 (1812)</t>
+  </si>
+  <si>
+    <t>12M Crystal (49UP)</t>
+  </si>
+  <si>
+    <t>Green LED (0603)</t>
+  </si>
+  <si>
+    <t>JTAG ARM connector (2x5 Box Header)</t>
+  </si>
+  <si>
+    <t>IC-Buck Converter (TPS62162DSGR)</t>
+  </si>
+  <si>
+    <t>IC-EEP_ROM (93LC56BT-I/OT)</t>
+  </si>
+  <si>
+    <t>IC-Isolator (ISO7231)</t>
+  </si>
+  <si>
+    <t>IC-USB to JTAG (FT2232H)</t>
+  </si>
+  <si>
+    <t>IC-Isolator</t>
+  </si>
+  <si>
+    <t>Item Number</t>
+  </si>
+  <si>
+    <t>IC-Isolator (ISO7240)</t>
   </si>
 </sst>
 </file>
@@ -1383,11 +1461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K22:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,21 +1479,22 @@
     <col min="7" max="7" width="20.33203125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="3.5546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1424,264 +1503,282 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>95</v>
-      </c>
-      <c r="O1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>97</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" t="s">
-        <v>139</v>
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N2">
+        <v>131</v>
+      </c>
+      <c r="N2" t="s">
+        <v>137</v>
+      </c>
+      <c r="O2">
         <v>0.1</v>
       </c>
-      <c r="O2">
-        <f>N2*C2</f>
+      <c r="P2">
+        <f t="shared" ref="P2:P26" si="0">O2*C2</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K3" t="s">
-        <v>141</v>
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="L3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="M3" t="s">
-        <v>140</v>
-      </c>
-      <c r="N3">
+        <v>131</v>
+      </c>
+      <c r="N3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O3">
         <v>0.1</v>
       </c>
-      <c r="O3">
-        <f>N3*C3</f>
+      <c r="P3">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
       <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K4" t="s">
-        <v>149</v>
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="L4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="M4" t="s">
-        <v>140</v>
-      </c>
-      <c r="N4">
+        <v>131</v>
+      </c>
+      <c r="N4" t="s">
+        <v>137</v>
+      </c>
+      <c r="O4">
         <v>0.1</v>
       </c>
-      <c r="O4">
-        <f>N4*C4</f>
+      <c r="P4">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
       <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K5" t="s">
-        <v>150</v>
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="M5" t="s">
-        <v>151</v>
-      </c>
-      <c r="N5">
+        <v>131</v>
+      </c>
+      <c r="N5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O5">
         <v>0.1</v>
       </c>
-      <c r="O5">
-        <f>N5*C5</f>
+      <c r="P5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
       <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="K6" t="s">
-        <v>152</v>
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="L6" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="M6" t="s">
-        <v>151</v>
-      </c>
-      <c r="N6">
+        <v>131</v>
+      </c>
+      <c r="N6" t="s">
+        <v>148</v>
+      </c>
+      <c r="O6">
         <v>0.1</v>
       </c>
-      <c r="O6">
-        <f>N6*C6</f>
+      <c r="P6">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1690,40 +1787,43 @@
         <v>330</v>
       </c>
       <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K7" t="s">
-        <v>156</v>
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="L7" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="M7" t="s">
-        <v>140</v>
-      </c>
-      <c r="N7">
+        <v>131</v>
+      </c>
+      <c r="N7" t="s">
+        <v>137</v>
+      </c>
+      <c r="O7">
         <v>0.1</v>
       </c>
-      <c r="O7">
-        <f>N7*C7</f>
+      <c r="P7">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1732,846 +1832,903 @@
         <v>820</v>
       </c>
       <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K8" t="s">
-        <v>160</v>
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="L8" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="M8" t="s">
-        <v>140</v>
-      </c>
-      <c r="N8">
+        <v>131</v>
+      </c>
+      <c r="N8" t="s">
+        <v>137</v>
+      </c>
+      <c r="O8">
         <v>0.1</v>
       </c>
-      <c r="O8">
-        <f>N8*C8</f>
+      <c r="P8">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K9" t="s">
-        <v>137</v>
+      <c r="J9" t="s">
+        <v>176</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="L9" t="s">
         <v>134</v>
       </c>
       <c r="M9" t="s">
-        <v>138</v>
-      </c>
-      <c r="N9">
+        <v>131</v>
+      </c>
+      <c r="N9" t="s">
+        <v>135</v>
+      </c>
+      <c r="O9">
         <v>0.1</v>
       </c>
-      <c r="O9">
-        <f>N9*C9</f>
+      <c r="P9">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K10" t="s">
-        <v>141</v>
+      <c r="J10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="L10" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="M10" t="s">
-        <v>142</v>
-      </c>
-      <c r="N10">
+        <v>131</v>
+      </c>
+      <c r="N10" t="s">
+        <v>139</v>
+      </c>
+      <c r="O10">
         <v>0.34</v>
       </c>
-      <c r="O10">
-        <f>N10*C10</f>
+      <c r="P10">
+        <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K11" t="s">
-        <v>154</v>
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>178</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="L11" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="M11" t="s">
-        <v>138</v>
-      </c>
-      <c r="N11">
+        <v>131</v>
+      </c>
+      <c r="N11" t="s">
+        <v>135</v>
+      </c>
+      <c r="O11">
         <v>0.48</v>
       </c>
-      <c r="O11">
-        <f>N11*C11</f>
+      <c r="P11">
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" t="s">
-        <v>155</v>
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="L12" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="M12" t="s">
-        <v>146</v>
-      </c>
-      <c r="N12">
+        <v>131</v>
+      </c>
+      <c r="N12" t="s">
+        <v>143</v>
+      </c>
+      <c r="O12">
         <v>0.36</v>
       </c>
-      <c r="O12">
-        <f>N12*C12</f>
+      <c r="P12">
+        <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K13" t="s">
-        <v>157</v>
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>180</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="L13" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="M13" t="s">
-        <v>143</v>
-      </c>
-      <c r="N13">
+        <v>131</v>
+      </c>
+      <c r="N13" t="s">
+        <v>140</v>
+      </c>
+      <c r="O13">
         <v>0.1</v>
       </c>
-      <c r="O13">
-        <f>N13*C13</f>
+      <c r="P13">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K14" t="s">
-        <v>158</v>
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="L14" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="M14" t="s">
-        <v>143</v>
-      </c>
-      <c r="N14">
+        <v>131</v>
+      </c>
+      <c r="N14" t="s">
+        <v>140</v>
+      </c>
+      <c r="O14">
         <v>0.4</v>
       </c>
-      <c r="O14">
-        <f>N14*C14</f>
+      <c r="P14">
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K15" t="s">
-        <v>153</v>
+      <c r="J15" t="s">
+        <v>182</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="L15" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="M15" t="s">
-        <v>146</v>
-      </c>
-      <c r="N15">
+        <v>131</v>
+      </c>
+      <c r="N15" t="s">
+        <v>143</v>
+      </c>
+      <c r="O15">
         <v>0.91</v>
       </c>
-      <c r="O15">
-        <f>N15*C15</f>
+      <c r="P15">
+        <f t="shared" si="0"/>
         <v>0.91</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>98</v>
+        <v>184</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>60</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>61</v>
       </c>
-      <c r="G16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16" t="s">
-        <v>159</v>
+      <c r="J16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N16">
+        <v>131</v>
+      </c>
+      <c r="N16" t="s">
+        <v>143</v>
+      </c>
+      <c r="O16">
         <v>0.25</v>
       </c>
-      <c r="O16">
-        <f>N16*C16</f>
+      <c r="P16">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>98</v>
+        <v>184</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
         <v>69</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" t="s">
         <v>70</v>
       </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" t="s">
-        <v>72</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K17" t="s">
-        <v>162</v>
+      <c r="J17" t="s">
+        <v>185</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="L17" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="M17" t="s">
-        <v>138</v>
-      </c>
-      <c r="N17">
+        <v>131</v>
+      </c>
+      <c r="N17" t="s">
+        <v>135</v>
+      </c>
+      <c r="O17">
         <v>0.1</v>
       </c>
-      <c r="O17">
-        <f>N17*C17</f>
+      <c r="P17">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>36</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>37</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>38</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
+        <v>187</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L18" t="s">
+        <v>144</v>
+      </c>
+      <c r="M18" t="s">
+        <v>131</v>
+      </c>
+      <c r="N18" t="s">
+        <v>145</v>
+      </c>
+      <c r="O18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R18" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K18" t="s">
-        <v>147</v>
-      </c>
-      <c r="L18" t="s">
-        <v>134</v>
-      </c>
-      <c r="M18" t="s">
-        <v>148</v>
-      </c>
-      <c r="N18">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="O18">
-        <f>N18*C18</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>40</v>
-      </c>
-      <c r="R18" t="s">
-        <v>40</v>
+      <c r="S18" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>13</v>
       </c>
-      <c r="H19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="J19" t="s">
+        <v>188</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L19" t="s">
+        <v>130</v>
+      </c>
+      <c r="M19" t="s">
+        <v>131</v>
+      </c>
+      <c r="N19" t="s">
         <v>133</v>
       </c>
-      <c r="L19" t="s">
-        <v>134</v>
-      </c>
-      <c r="M19" t="s">
-        <v>136</v>
-      </c>
-      <c r="N19">
+      <c r="O19">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O19">
-        <f>N19*C19</f>
+      <c r="P19">
+        <f t="shared" si="0"/>
         <v>0.86999999999999988</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
         <v>32</v>
       </c>
-      <c r="E20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>33</v>
       </c>
-      <c r="G20" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K20" t="s">
-        <v>32</v>
+      <c r="J20" t="s">
+        <v>189</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="L20" t="s">
-        <v>134</v>
+        <v>31</v>
       </c>
       <c r="M20" t="s">
-        <v>145</v>
-      </c>
-      <c r="N20">
+        <v>131</v>
+      </c>
+      <c r="N20" t="s">
+        <v>142</v>
+      </c>
+      <c r="O20">
         <v>0.51</v>
       </c>
-      <c r="O20">
-        <f>N20*C20</f>
+      <c r="P20">
+        <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>88</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>89</v>
       </c>
-      <c r="G21" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" t="s">
+        <v>127</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L21" t="s">
+        <v>166</v>
+      </c>
+      <c r="M21" t="s">
         <v>131</v>
       </c>
-      <c r="K21" t="s">
-        <v>169</v>
-      </c>
-      <c r="L21" t="s">
-        <v>134</v>
-      </c>
-      <c r="M21" t="s">
-        <v>166</v>
-      </c>
-      <c r="N21">
+      <c r="N21" t="s">
+        <v>163</v>
+      </c>
+      <c r="O21">
         <v>0.71</v>
       </c>
-      <c r="O21">
-        <f>N21*C21</f>
+      <c r="P21">
+        <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
-      <c r="Q21" t="s">
-        <v>40</v>
-      </c>
       <c r="R21" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="S21" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" t="s">
         <v>84</v>
       </c>
-      <c r="E22" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" t="s">
-        <v>86</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" t="s">
+        <v>190</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22" t="s">
+        <v>165</v>
+      </c>
+      <c r="M22" t="s">
+        <v>131</v>
+      </c>
+      <c r="N22" t="s">
+        <v>163</v>
+      </c>
+      <c r="O22">
+        <v>1.91</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>129</v>
       </c>
-      <c r="K22" t="s">
-        <v>168</v>
-      </c>
-      <c r="L22" t="s">
-        <v>134</v>
-      </c>
-      <c r="M22" t="s">
-        <v>166</v>
-      </c>
-      <c r="N22">
-        <v>1.91</v>
-      </c>
-      <c r="O22">
-        <f>N22*C22</f>
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>132</v>
-      </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E23">
         <v>93</v>
       </c>
       <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" t="s">
         <v>66</v>
       </c>
-      <c r="G23" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K23" t="s">
-        <v>161</v>
+      <c r="J23" t="s">
+        <v>191</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="L23" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="M23" t="s">
-        <v>144</v>
-      </c>
-      <c r="N23">
+        <v>131</v>
+      </c>
+      <c r="N23" t="s">
+        <v>141</v>
+      </c>
+      <c r="O23">
         <v>0.28000000000000003</v>
       </c>
-      <c r="O23">
-        <f>N23*C23</f>
+      <c r="P23">
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
         <v>76</v>
       </c>
-      <c r="E24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K24" t="s">
-        <v>165</v>
+      <c r="J24" t="s">
+        <v>192</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="L24" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="M24" t="s">
-        <v>166</v>
-      </c>
-      <c r="N24">
+        <v>131</v>
+      </c>
+      <c r="N24" t="s">
+        <v>163</v>
+      </c>
+      <c r="O24">
         <v>3.96</v>
       </c>
-      <c r="O24">
-        <f>N24*C24</f>
+      <c r="P24">
+        <f t="shared" si="0"/>
         <v>3.96</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" t="s">
         <v>79</v>
       </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
+        <v>196</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L25" t="s">
+        <v>164</v>
+      </c>
+      <c r="M25" t="s">
+        <v>131</v>
+      </c>
+      <c r="N25" t="s">
+        <v>163</v>
+      </c>
+      <c r="O25">
+        <v>5.09</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>5.09</v>
+      </c>
+      <c r="Q25" t="s">
         <v>80</v>
       </c>
-      <c r="H25" t="s">
+      <c r="R25">
+        <v>1755124</v>
+      </c>
+      <c r="S25" t="s">
         <v>81</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K25" t="s">
-        <v>167</v>
-      </c>
-      <c r="L25" t="s">
-        <v>134</v>
-      </c>
-      <c r="M25" t="s">
-        <v>166</v>
-      </c>
-      <c r="N25">
-        <v>5.09</v>
-      </c>
-      <c r="O25">
-        <f>N25*C25</f>
-        <v>5.09</v>
-      </c>
-      <c r="P25" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q25">
-        <v>1755124</v>
-      </c>
-      <c r="R25" t="s">
-        <v>83</v>
-      </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" t="s">
         <v>73</v>
       </c>
-      <c r="E26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K26" t="s">
-        <v>163</v>
+      <c r="J26" t="s">
+        <v>193</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="L26" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="M26" t="s">
-        <v>164</v>
-      </c>
-      <c r="N26">
+        <v>131</v>
+      </c>
+      <c r="N26" t="s">
+        <v>161</v>
+      </c>
+      <c r="O26">
         <v>6.71</v>
       </c>
-      <c r="O26">
-        <f>N26*C26</f>
+      <c r="P26">
+        <f t="shared" si="0"/>
         <v>6.71</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="O27">
-        <f>SUM(O9:O26)</f>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <f>SUM(P9:P26)</f>
         <v>24.36</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A9:S28">
+  <sortState ref="A9:T28">
     <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="J19" r:id="rId1" xr:uid="{040F2726-1D90-4856-936E-81EF30FFA10A}"/>
-    <hyperlink ref="J9" r:id="rId2" xr:uid="{1347D1DE-BAD0-420A-A040-3E6433E78833}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{951F61AC-B0DA-4F32-8B55-7C19A8C7980B}"/>
-    <hyperlink ref="J3" r:id="rId4" xr:uid="{86E4D402-9609-4039-89D1-569AF33AE939}"/>
-    <hyperlink ref="J20" r:id="rId5" xr:uid="{1857F071-0672-4A1E-A656-D05C09A54542}"/>
-    <hyperlink ref="J10" r:id="rId6" xr:uid="{34161D84-8245-40A2-A3D1-E9E58CA76FD4}"/>
-    <hyperlink ref="J4" r:id="rId7" xr:uid="{22D6C509-F57B-4741-BBF2-916A4AEA7F9D}"/>
-    <hyperlink ref="J5" r:id="rId8" xr:uid="{E9D70A45-ECBA-4402-8B0B-3A5BB1B1AECE}"/>
-    <hyperlink ref="J15" r:id="rId9" xr:uid="{F600E220-0B81-4D3C-801D-3BD723591713}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{316A640C-4115-4C02-A9EA-40A1634919A5}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{AB210E39-BB8A-40D1-9B07-CD96AA50B94C}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{C0E554F9-7151-437B-8C8E-C2A641D6D1BD}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{59B34D7F-DAC4-4C4E-A20C-1631F068BAE5}"/>
-    <hyperlink ref="J16" r:id="rId14" xr:uid="{01D88F47-4C5D-4021-B9AF-1339A7B317F1}"/>
-    <hyperlink ref="J8" r:id="rId15" xr:uid="{59EEDD7D-EA24-46E8-85AE-7CFA74AFC155}"/>
-    <hyperlink ref="J23" r:id="rId16" xr:uid="{61A9B3EC-C738-44C1-AD90-0247FA16D92D}"/>
-    <hyperlink ref="J17" r:id="rId17" xr:uid="{4C4FA93E-C297-40F0-8B91-9D6AB4314CDF}"/>
-    <hyperlink ref="J26" r:id="rId18" xr:uid="{221C5FC6-5A71-49BF-8587-5C4FF61FA0F5}"/>
-    <hyperlink ref="J24" r:id="rId19" xr:uid="{7DBF3B77-257A-4F9D-B700-1D5F645DD93C}"/>
-    <hyperlink ref="J25" r:id="rId20" xr:uid="{12217847-3FC7-43CE-BC70-89AB72680EF1}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{BDEA88A0-5765-4375-BC16-869A45C92963}"/>
-    <hyperlink ref="J18" r:id="rId22" xr:uid="{7D0FF286-90AB-4B80-8BC5-67A08AE6A0FF}"/>
-    <hyperlink ref="J6" r:id="rId23" xr:uid="{61557CCD-7865-4BD0-9177-C3422D2BFD8B}"/>
-    <hyperlink ref="J7" r:id="rId24" xr:uid="{D8396314-4822-4914-B3B9-6FDB04DF42F3}"/>
+    <hyperlink ref="K19" r:id="rId1" xr:uid="{040F2726-1D90-4856-936E-81EF30FFA10A}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{1347D1DE-BAD0-420A-A040-3E6433E78833}"/>
+    <hyperlink ref="K2" r:id="rId3" xr:uid="{951F61AC-B0DA-4F32-8B55-7C19A8C7980B}"/>
+    <hyperlink ref="K3" r:id="rId4" xr:uid="{86E4D402-9609-4039-89D1-569AF33AE939}"/>
+    <hyperlink ref="K20" r:id="rId5" xr:uid="{1857F071-0672-4A1E-A656-D05C09A54542}"/>
+    <hyperlink ref="K10" r:id="rId6" xr:uid="{34161D84-8245-40A2-A3D1-E9E58CA76FD4}"/>
+    <hyperlink ref="K4" r:id="rId7" xr:uid="{22D6C509-F57B-4741-BBF2-916A4AEA7F9D}"/>
+    <hyperlink ref="K5" r:id="rId8" xr:uid="{E9D70A45-ECBA-4402-8B0B-3A5BB1B1AECE}"/>
+    <hyperlink ref="K15" r:id="rId9" xr:uid="{F600E220-0B81-4D3C-801D-3BD723591713}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{316A640C-4115-4C02-A9EA-40A1634919A5}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{AB210E39-BB8A-40D1-9B07-CD96AA50B94C}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{C0E554F9-7151-437B-8C8E-C2A641D6D1BD}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{59B34D7F-DAC4-4C4E-A20C-1631F068BAE5}"/>
+    <hyperlink ref="K16" r:id="rId14" xr:uid="{01D88F47-4C5D-4021-B9AF-1339A7B317F1}"/>
+    <hyperlink ref="K8" r:id="rId15" xr:uid="{59EEDD7D-EA24-46E8-85AE-7CFA74AFC155}"/>
+    <hyperlink ref="K23" r:id="rId16" xr:uid="{61A9B3EC-C738-44C1-AD90-0247FA16D92D}"/>
+    <hyperlink ref="K17" r:id="rId17" xr:uid="{4C4FA93E-C297-40F0-8B91-9D6AB4314CDF}"/>
+    <hyperlink ref="K26" r:id="rId18" xr:uid="{221C5FC6-5A71-49BF-8587-5C4FF61FA0F5}"/>
+    <hyperlink ref="K24" r:id="rId19" xr:uid="{7DBF3B77-257A-4F9D-B700-1D5F645DD93C}"/>
+    <hyperlink ref="K25" r:id="rId20" xr:uid="{12217847-3FC7-43CE-BC70-89AB72680EF1}"/>
+    <hyperlink ref="K22" r:id="rId21" xr:uid="{BDEA88A0-5765-4375-BC16-869A45C92963}"/>
+    <hyperlink ref="K18" r:id="rId22" xr:uid="{7D0FF286-90AB-4B80-8BC5-67A08AE6A0FF}"/>
+    <hyperlink ref="K6" r:id="rId23" xr:uid="{61557CCD-7865-4BD0-9177-C3422D2BFD8B}"/>
+    <hyperlink ref="K7" r:id="rId24" xr:uid="{D8396314-4822-4914-B3B9-6FDB04DF42F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId25"/>

</xml_diff>

<commit_message>
Changed footprint of FTDI chip
The solder pads were too close to the chip, and as such most of the pad was underneath the chip. The pads were moved and the circuit modified.
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1463,9 +1463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K22:K26"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>